<commit_message>
Updated plot and change latitude to abs value
</commit_message>
<xml_diff>
--- a/Data/meta_analysis.xlsx
+++ b/Data/meta_analysis.xlsx
@@ -4236,7 +4236,7 @@
     <t xml:space="preserve">inferred from Fig. 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Aselluls </t>
+    <t xml:space="preserve">Aselluls</t>
   </si>
   <si>
     <t xml:space="preserve">aquaticus carniolicus</t>
@@ -5162,11 +5162,11 @@
   <dimension ref="A1:R995"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
+      <selection pane="bottomRight" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11110,15 +11110,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB350"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A353" activeCellId="0" sqref="A353"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="bottomLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11236,7 +11236,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
@@ -11323,7 +11323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
         <v>18</v>
       </c>
@@ -11410,7 +11410,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
@@ -11497,7 +11497,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
         <v>18</v>
       </c>
@@ -11584,7 +11584,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
         <v>18</v>
       </c>
@@ -11671,7 +11671,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
         <v>18</v>
       </c>
@@ -11758,7 +11758,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
         <v>18</v>
       </c>
@@ -11845,7 +11845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
         <v>18</v>
       </c>
@@ -11932,7 +11932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
         <v>18</v>
       </c>
@@ -12019,7 +12019,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
         <v>18</v>
       </c>
@@ -12106,7 +12106,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
         <v>18</v>
       </c>
@@ -12193,7 +12193,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
         <v>18</v>
       </c>
@@ -12280,7 +12280,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
         <v>18</v>
       </c>
@@ -12367,7 +12367,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
         <v>18</v>
       </c>
@@ -12454,7 +12454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
         <v>40</v>
       </c>
@@ -12541,7 +12541,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
         <v>40</v>
       </c>
@@ -12628,7 +12628,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
         <v>40</v>
       </c>
@@ -12715,7 +12715,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
         <v>40</v>
       </c>
@@ -12802,7 +12802,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
         <v>58</v>
       </c>
@@ -12889,7 +12889,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="20" t="s">
         <v>58</v>
       </c>
@@ -12976,7 +12976,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="20" t="s">
         <v>64</v>
       </c>
@@ -13063,7 +13063,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="20" t="s">
         <v>64</v>
       </c>
@@ -13150,7 +13150,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="20" t="s">
         <v>64</v>
       </c>
@@ -13237,7 +13237,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="20" t="s">
         <v>64</v>
       </c>
@@ -13324,7 +13324,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="20" t="s">
         <v>72</v>
       </c>
@@ -13408,7 +13408,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="20" t="s">
         <v>72</v>
       </c>
@@ -13492,7 +13492,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="20" t="s">
         <v>72</v>
       </c>
@@ -13576,7 +13576,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="20" t="s">
         <v>72</v>
       </c>
@@ -13663,7 +13663,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="20" t="s">
         <v>72</v>
       </c>
@@ -13750,7 +13750,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="20" t="s">
         <v>72</v>
       </c>
@@ -13834,7 +13834,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="20" t="s">
         <v>79</v>
       </c>
@@ -13921,7 +13921,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="20" t="s">
         <v>79</v>
       </c>
@@ -14009,7 +14009,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="20" t="s">
         <v>79</v>
       </c>
@@ -14096,7 +14096,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="20" t="s">
         <v>79</v>
       </c>
@@ -14184,7 +14184,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="20" t="s">
         <v>79</v>
       </c>
@@ -14271,7 +14271,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="20" t="s">
         <v>79</v>
       </c>
@@ -14359,7 +14359,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>88</v>
       </c>
@@ -14446,7 +14446,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>88</v>
       </c>
@@ -14533,7 +14533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>88</v>
       </c>
@@ -14620,7 +14620,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>88</v>
       </c>
@@ -14707,7 +14707,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>88</v>
       </c>
@@ -14794,7 +14794,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>88</v>
       </c>
@@ -14881,7 +14881,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>88</v>
       </c>
@@ -14968,7 +14968,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -15055,7 +15055,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>95</v>
       </c>
@@ -15141,7 +15141,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>95</v>
       </c>
@@ -15227,7 +15227,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>95</v>
       </c>
@@ -15313,7 +15313,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>95</v>
       </c>
@@ -15399,7 +15399,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="20" t="s">
         <v>105</v>
       </c>
@@ -15487,7 +15487,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="20" t="s">
         <v>105</v>
       </c>
@@ -15575,7 +15575,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="20" t="s">
         <v>111</v>
       </c>
@@ -15663,7 +15663,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="20" t="s">
         <v>116</v>
       </c>
@@ -15749,7 +15749,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="20" t="s">
         <v>116</v>
       </c>
@@ -15835,7 +15835,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="20" t="s">
         <v>116</v>
       </c>
@@ -15921,7 +15921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="20" t="s">
         <v>116</v>
       </c>
@@ -16007,7 +16007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="20" t="s">
         <v>116</v>
       </c>
@@ -16093,7 +16093,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="20" t="s">
         <v>116</v>
       </c>
@@ -16179,7 +16179,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="20" t="s">
         <v>116</v>
       </c>
@@ -16265,7 +16265,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="20" t="s">
         <v>116</v>
       </c>
@@ -16351,7 +16351,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>124</v>
       </c>
@@ -16437,7 +16437,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>124</v>
       </c>
@@ -16523,7 +16523,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>124</v>
       </c>
@@ -16609,7 +16609,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>124</v>
       </c>
@@ -16695,7 +16695,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>124</v>
       </c>
@@ -16781,7 +16781,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>124</v>
       </c>
@@ -16867,7 +16867,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>124</v>
       </c>
@@ -16953,7 +16953,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>124</v>
       </c>
@@ -17039,7 +17039,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="20" t="s">
         <v>130</v>
       </c>
@@ -17126,7 +17126,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="20" t="s">
         <v>130</v>
       </c>
@@ -17213,7 +17213,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="20" t="s">
         <v>130</v>
       </c>
@@ -17300,7 +17300,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="20" t="s">
         <v>130</v>
       </c>
@@ -17387,7 +17387,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="20" t="s">
         <v>130</v>
       </c>
@@ -17474,7 +17474,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="20" t="s">
         <v>130</v>
       </c>
@@ -17561,7 +17561,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="20" t="s">
         <v>130</v>
       </c>
@@ -17648,7 +17648,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="20" t="s">
         <v>130</v>
       </c>
@@ -17735,7 +17735,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="20" t="s">
         <v>130</v>
       </c>
@@ -17822,7 +17822,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="20" t="s">
         <v>130</v>
       </c>
@@ -17909,7 +17909,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="20" t="s">
         <v>130</v>
       </c>
@@ -17996,7 +17996,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="20" t="s">
         <v>130</v>
       </c>
@@ -18083,7 +18083,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="20" t="s">
         <v>130</v>
       </c>
@@ -18170,7 +18170,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="20" t="s">
         <v>130</v>
       </c>
@@ -18257,7 +18257,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="20" t="s">
         <v>130</v>
       </c>
@@ -18344,7 +18344,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="20" t="s">
         <v>130</v>
       </c>
@@ -18431,7 +18431,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="20" t="s">
         <v>138</v>
       </c>
@@ -18518,7 +18518,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="20" t="s">
         <v>138</v>
       </c>
@@ -18605,7 +18605,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="20" t="s">
         <v>138</v>
       </c>
@@ -18692,7 +18692,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="20" t="s">
         <v>138</v>
       </c>
@@ -18779,7 +18779,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="20" t="s">
         <v>138</v>
       </c>
@@ -18866,7 +18866,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="20" t="s">
         <v>138</v>
       </c>
@@ -18953,7 +18953,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="20" t="s">
         <v>138</v>
       </c>
@@ -19040,7 +19040,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="20" t="s">
         <v>138</v>
       </c>
@@ -19127,7 +19127,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="20" t="s">
         <v>138</v>
       </c>
@@ -19214,7 +19214,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="20" t="s">
         <v>138</v>
       </c>
@@ -19301,7 +19301,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="20" t="s">
         <v>138</v>
       </c>
@@ -19388,7 +19388,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="20" t="s">
         <v>138</v>
       </c>
@@ -19475,7 +19475,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="20" t="s">
         <v>144</v>
       </c>
@@ -19559,7 +19559,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="20" t="s">
         <v>144</v>
       </c>
@@ -19643,7 +19643,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="20" t="s">
         <v>144</v>
       </c>
@@ -19727,7 +19727,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="20" t="s">
         <v>149</v>
       </c>
@@ -19814,7 +19814,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="20" t="s">
         <v>155</v>
       </c>
@@ -19901,7 +19901,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="20" t="s">
         <v>155</v>
       </c>
@@ -19988,7 +19988,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="20" t="s">
         <v>160</v>
       </c>
@@ -20075,7 +20075,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="20" t="s">
         <v>160</v>
       </c>
@@ -20162,7 +20162,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="20" t="s">
         <v>160</v>
       </c>
@@ -20249,7 +20249,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="20" t="s">
         <v>160</v>
       </c>
@@ -20336,7 +20336,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="20" t="s">
         <v>160</v>
       </c>
@@ -20423,7 +20423,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="20" t="s">
         <v>160</v>
       </c>
@@ -20510,7 +20510,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="20" t="s">
         <v>165</v>
       </c>
@@ -20597,7 +20597,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="20" t="s">
         <v>165</v>
       </c>
@@ -20684,7 +20684,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="20" t="s">
         <v>165</v>
       </c>
@@ -20771,7 +20771,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
         <v>171</v>
       </c>
@@ -20858,7 +20858,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
         <v>171</v>
       </c>
@@ -20945,7 +20945,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
         <v>171</v>
       </c>
@@ -21032,7 +21032,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
         <v>171</v>
       </c>
@@ -21119,7 +21119,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
         <v>171</v>
       </c>
@@ -21205,7 +21205,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
         <v>171</v>
       </c>
@@ -21291,7 +21291,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
         <v>171</v>
       </c>
@@ -21377,7 +21377,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
         <v>171</v>
       </c>
@@ -21463,7 +21463,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="20" t="s">
         <v>185</v>
       </c>
@@ -21550,7 +21550,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="20" t="s">
         <v>185</v>
       </c>
@@ -21637,7 +21637,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="20" t="s">
         <v>185</v>
       </c>
@@ -21724,7 +21724,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="20" t="s">
         <v>185</v>
       </c>
@@ -21811,7 +21811,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="20" t="s">
         <v>185</v>
       </c>
@@ -21898,7 +21898,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="20" t="s">
         <v>185</v>
       </c>
@@ -21985,7 +21985,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="20" t="s">
         <v>185</v>
       </c>
@@ -22072,7 +22072,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="20" t="s">
         <v>185</v>
       </c>
@@ -22159,7 +22159,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="20" t="s">
         <v>185</v>
       </c>
@@ -22246,7 +22246,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="20" t="s">
         <v>185</v>
       </c>
@@ -22333,7 +22333,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="20" t="s">
         <v>185</v>
       </c>
@@ -22420,7 +22420,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="20" t="s">
         <v>185</v>
       </c>
@@ -22507,7 +22507,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="20" t="s">
         <v>185</v>
       </c>
@@ -22594,7 +22594,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="20" t="s">
         <v>185</v>
       </c>
@@ -22681,7 +22681,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="20" t="s">
         <v>185</v>
       </c>
@@ -22768,7 +22768,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="20" t="s">
         <v>185</v>
       </c>
@@ -22941,7 +22941,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="20" t="s">
         <v>198</v>
       </c>
@@ -23028,7 +23028,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="20" t="s">
         <v>198</v>
       </c>
@@ -23115,7 +23115,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="20" t="s">
         <v>198</v>
       </c>
@@ -23202,7 +23202,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="20" t="s">
         <v>198</v>
       </c>
@@ -23289,7 +23289,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="20" t="s">
         <v>198</v>
       </c>
@@ -23376,7 +23376,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="20" t="s">
         <v>198</v>
       </c>
@@ -23463,7 +23463,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="20" t="s">
         <v>204</v>
       </c>
@@ -23549,7 +23549,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="20" t="s">
         <v>212</v>
       </c>
@@ -23636,7 +23636,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="20" t="s">
         <v>212</v>
       </c>
@@ -23723,7 +23723,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="20" t="s">
         <v>218</v>
       </c>
@@ -23810,7 +23810,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="20" t="s">
         <v>218</v>
       </c>
@@ -23897,7 +23897,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="20" t="s">
         <v>223</v>
       </c>
@@ -23984,7 +23984,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="20" t="s">
         <v>223</v>
       </c>
@@ -24071,7 +24071,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="20" t="s">
         <v>223</v>
       </c>
@@ -24158,7 +24158,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="20" t="s">
         <v>223</v>
       </c>
@@ -24245,7 +24245,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="20" t="s">
         <v>223</v>
       </c>
@@ -24332,7 +24332,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="20" t="s">
         <v>231</v>
       </c>
@@ -24418,7 +24418,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="20" t="s">
         <v>231</v>
       </c>
@@ -24504,7 +24504,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="20" t="s">
         <v>231</v>
       </c>
@@ -24590,7 +24590,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="20" t="s">
         <v>237</v>
       </c>
@@ -24677,7 +24677,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="32" t="s">
         <v>244</v>
       </c>
@@ -24763,7 +24763,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="32" t="s">
         <v>250</v>
       </c>
@@ -24849,7 +24849,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="32" t="s">
         <v>250</v>
       </c>
@@ -24935,7 +24935,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="32" t="s">
         <v>258</v>
       </c>
@@ -25021,7 +25021,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="32" t="s">
         <v>258</v>
       </c>
@@ -25107,7 +25107,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="32" t="s">
         <v>882</v>
       </c>
@@ -25193,7 +25193,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="32" t="s">
         <v>264</v>
       </c>
@@ -25280,7 +25280,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="32" t="s">
         <v>264</v>
       </c>
@@ -25367,7 +25367,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="32" t="s">
         <v>264</v>
       </c>
@@ -25454,7 +25454,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="32" t="s">
         <v>264</v>
       </c>
@@ -25541,7 +25541,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="32" t="s">
         <v>264</v>
       </c>
@@ -25627,7 +25627,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="32" t="s">
         <v>264</v>
       </c>
@@ -25713,7 +25713,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="32" t="s">
         <v>264</v>
       </c>
@@ -25800,7 +25800,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="32" t="s">
         <v>264</v>
       </c>
@@ -25887,7 +25887,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="32" t="s">
         <v>264</v>
       </c>
@@ -25974,7 +25974,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="32" t="s">
         <v>264</v>
       </c>
@@ -26061,7 +26061,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="32" t="s">
         <v>264</v>
       </c>
@@ -26147,7 +26147,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="32" t="s">
         <v>264</v>
       </c>
@@ -26233,7 +26233,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="32" t="s">
         <v>264</v>
       </c>
@@ -26319,7 +26319,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="32" t="s">
         <v>264</v>
       </c>
@@ -26405,7 +26405,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="32" t="s">
         <v>264</v>
       </c>
@@ -26921,7 +26921,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="32" t="s">
         <v>276</v>
       </c>
@@ -27007,7 +27007,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="32" t="s">
         <v>276</v>
       </c>
@@ -27093,7 +27093,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="32" t="s">
         <v>276</v>
       </c>
@@ -27179,7 +27179,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="32" t="s">
         <v>276</v>
       </c>
@@ -27265,7 +27265,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="29" t="s">
         <v>282</v>
       </c>
@@ -27351,7 +27351,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="29" t="s">
         <v>282</v>
       </c>
@@ -27437,7 +27437,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="20" t="s">
         <v>288</v>
       </c>
@@ -27524,7 +27524,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="20" t="s">
         <v>288</v>
       </c>
@@ -27611,7 +27611,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="20" t="s">
         <v>302</v>
       </c>
@@ -27698,7 +27698,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="20" t="s">
         <v>302</v>
       </c>
@@ -27785,7 +27785,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="20" t="s">
         <v>308</v>
       </c>
@@ -27872,7 +27872,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="20" t="s">
         <v>308</v>
       </c>
@@ -27959,7 +27959,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="20" t="s">
         <v>308</v>
       </c>
@@ -28046,7 +28046,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="20" t="s">
         <v>308</v>
       </c>
@@ -28133,7 +28133,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="20" t="s">
         <v>327</v>
       </c>
@@ -28219,7 +28219,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="20" t="s">
         <v>327</v>
       </c>
@@ -28305,7 +28305,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="20" t="s">
         <v>327</v>
       </c>
@@ -28391,7 +28391,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="20" t="s">
         <v>327</v>
       </c>
@@ -28478,7 +28478,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="20" t="s">
         <v>327</v>
       </c>
@@ -28564,7 +28564,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="20" t="s">
         <v>327</v>
       </c>
@@ -28651,7 +28651,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="20" t="s">
         <v>327</v>
       </c>
@@ -28737,7 +28737,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="20" t="s">
         <v>327</v>
       </c>
@@ -28823,7 +28823,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="20" t="s">
         <v>333</v>
       </c>
@@ -28909,7 +28909,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="20" t="s">
         <v>333</v>
       </c>
@@ -28995,7 +28995,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="20" t="s">
         <v>333</v>
       </c>
@@ -29081,7 +29081,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="20" t="s">
         <v>339</v>
       </c>
@@ -29167,7 +29167,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="20" t="s">
         <v>339</v>
       </c>
@@ -29253,7 +29253,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="20" t="s">
         <v>339</v>
       </c>
@@ -29339,7 +29339,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="20" t="s">
         <v>339</v>
       </c>
@@ -29425,7 +29425,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="20" t="s">
         <v>339</v>
       </c>
@@ -29511,7 +29511,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="20" t="s">
         <v>345</v>
       </c>
@@ -29597,7 +29597,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="20" t="s">
         <v>345</v>
       </c>
@@ -29683,7 +29683,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="20" t="s">
         <v>351</v>
       </c>
@@ -29769,7 +29769,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="20" t="s">
         <v>364</v>
       </c>
@@ -29855,7 +29855,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="20" t="s">
         <v>364</v>
       </c>
@@ -29941,7 +29941,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="20" t="s">
         <v>364</v>
       </c>
@@ -30027,7 +30027,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="20" t="s">
         <v>364</v>
       </c>
@@ -30113,7 +30113,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="20" t="s">
         <v>364</v>
       </c>
@@ -30199,7 +30199,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="20" t="s">
         <v>364</v>
       </c>
@@ -30285,7 +30285,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="20" t="s">
         <v>364</v>
       </c>
@@ -30371,7 +30371,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="20" t="s">
         <v>364</v>
       </c>
@@ -30457,7 +30457,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="20" t="s">
         <v>364</v>
       </c>
@@ -30543,7 +30543,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="20" t="s">
         <v>370</v>
       </c>
@@ -30629,7 +30629,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="20" t="s">
         <v>376</v>
       </c>
@@ -30715,7 +30715,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="20" t="s">
         <v>382</v>
       </c>
@@ -30801,7 +30801,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="20" t="s">
         <v>382</v>
       </c>
@@ -30887,7 +30887,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="20" t="s">
         <v>382</v>
       </c>
@@ -30973,7 +30973,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="20" t="s">
         <v>389</v>
       </c>
@@ -31059,7 +31059,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="20" t="s">
         <v>389</v>
       </c>
@@ -31145,7 +31145,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="20" t="s">
         <v>389</v>
       </c>
@@ -31231,7 +31231,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="20" t="s">
         <v>395</v>
       </c>
@@ -31317,7 +31317,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="20" t="s">
         <v>395</v>
       </c>
@@ -31403,7 +31403,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="20" t="s">
         <v>395</v>
       </c>
@@ -31489,7 +31489,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="20" t="s">
         <v>395</v>
       </c>
@@ -31575,7 +31575,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="20" t="s">
         <v>395</v>
       </c>
@@ -31661,7 +31661,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="20" t="s">
         <v>395</v>
       </c>
@@ -31747,7 +31747,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="20" t="s">
         <v>401</v>
       </c>
@@ -31833,7 +31833,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="20" t="s">
         <v>401</v>
       </c>
@@ -31919,7 +31919,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="20" t="s">
         <v>401</v>
       </c>
@@ -32005,7 +32005,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="20" t="s">
         <v>401</v>
       </c>
@@ -32091,7 +32091,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="20" t="s">
         <v>401</v>
       </c>
@@ -32177,7 +32177,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="20" t="s">
         <v>406</v>
       </c>
@@ -32263,7 +32263,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="20" t="s">
         <v>406</v>
       </c>
@@ -32349,7 +32349,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="20" t="s">
         <v>406</v>
       </c>
@@ -32435,7 +32435,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="20" t="s">
         <v>412</v>
       </c>
@@ -32521,7 +32521,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="20" t="s">
         <v>417</v>
       </c>
@@ -32608,7 +32608,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="249" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="20" t="s">
         <v>417</v>
       </c>
@@ -32695,7 +32695,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="250" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="20" t="s">
         <v>417</v>
       </c>
@@ -32782,7 +32782,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="20" t="s">
         <v>417</v>
       </c>
@@ -32869,7 +32869,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="20" t="s">
         <v>417</v>
       </c>
@@ -32956,7 +32956,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="20" t="s">
         <v>417</v>
       </c>
@@ -33043,7 +33043,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="20" t="s">
         <v>417</v>
       </c>
@@ -33130,7 +33130,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="20" t="s">
         <v>417</v>
       </c>
@@ -33217,7 +33217,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="20" t="s">
         <v>417</v>
       </c>
@@ -33304,7 +33304,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A257" s="20" t="s">
         <v>417</v>
       </c>
@@ -33391,7 +33391,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A258" s="20" t="s">
         <v>417</v>
       </c>
@@ -33478,7 +33478,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A259" s="20" t="s">
         <v>417</v>
       </c>
@@ -33565,7 +33565,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A260" s="20" t="s">
         <v>417</v>
       </c>
@@ -33652,7 +33652,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A261" s="20" t="s">
         <v>417</v>
       </c>
@@ -33739,7 +33739,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A262" s="20" t="s">
         <v>417</v>
       </c>
@@ -33826,7 +33826,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A263" s="20" t="s">
         <v>424</v>
       </c>
@@ -33913,7 +33913,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A264" s="20" t="s">
         <v>431</v>
       </c>
@@ -34000,7 +34000,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A265" s="20" t="s">
         <v>431</v>
       </c>
@@ -34087,7 +34087,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A266" s="20" t="s">
         <v>437</v>
       </c>
@@ -34174,7 +34174,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A267" s="2" t="s">
         <v>443</v>
       </c>
@@ -34260,7 +34260,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
         <v>443</v>
       </c>
@@ -34346,7 +34346,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A269" s="2" t="s">
         <v>443</v>
       </c>
@@ -34432,7 +34432,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
         <v>443</v>
       </c>
@@ -34518,7 +34518,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A271" s="2" t="s">
         <v>443</v>
       </c>
@@ -34604,7 +34604,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A272" s="2" t="s">
         <v>443</v>
       </c>
@@ -34690,7 +34690,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A273" s="2" t="s">
         <v>443</v>
       </c>
@@ -34776,7 +34776,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="2" t="s">
         <v>443</v>
       </c>
@@ -34862,7 +34862,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
         <v>443</v>
       </c>
@@ -34948,7 +34948,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
         <v>443</v>
       </c>
@@ -35034,7 +35034,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
         <v>443</v>
       </c>
@@ -35120,7 +35120,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
         <v>443</v>
       </c>
@@ -35206,7 +35206,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="279" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A279" s="20" t="s">
         <v>448</v>
       </c>
@@ -35293,7 +35293,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A280" s="20" t="s">
         <v>448</v>
       </c>
@@ -35380,7 +35380,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="281" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A281" s="20" t="s">
         <v>448</v>
       </c>
@@ -35467,7 +35467,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="282" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A282" s="20" t="s">
         <v>448</v>
       </c>
@@ -35554,7 +35554,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="283" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A283" s="20" t="s">
         <v>448</v>
       </c>
@@ -35641,7 +35641,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A284" s="20" t="s">
         <v>448</v>
       </c>
@@ -35728,7 +35728,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="285" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A285" s="20" t="s">
         <v>448</v>
       </c>
@@ -35814,7 +35814,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A286" s="20" t="s">
         <v>448</v>
       </c>
@@ -35900,7 +35900,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A287" s="20" t="s">
         <v>455</v>
       </c>
@@ -35987,7 +35987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A288" s="20" t="s">
         <v>455</v>
       </c>
@@ -36074,7 +36074,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A289" s="20" t="s">
         <v>455</v>
       </c>
@@ -36161,7 +36161,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="290" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A290" s="20" t="s">
         <v>455</v>
       </c>
@@ -36248,7 +36248,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="291" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A291" s="20" t="s">
         <v>462</v>
       </c>
@@ -36335,7 +36335,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A292" s="20" t="s">
         <v>462</v>
       </c>
@@ -36422,7 +36422,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="293" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A293" s="20" t="s">
         <v>462</v>
       </c>
@@ -36509,7 +36509,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="294" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A294" s="20" t="s">
         <v>462</v>
       </c>
@@ -36596,7 +36596,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A295" s="20" t="s">
         <v>462</v>
       </c>
@@ -36683,7 +36683,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A296" s="20" t="s">
         <v>462</v>
       </c>
@@ -37034,7 +37034,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="20" t="s">
         <v>471</v>
       </c>
@@ -37122,7 +37122,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="20" t="s">
         <v>471</v>
       </c>
@@ -37210,7 +37210,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A302" s="20" t="s">
         <v>471</v>
       </c>
@@ -37298,7 +37298,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="20" t="s">
         <v>471</v>
       </c>
@@ -37386,7 +37386,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A304" s="20" t="s">
         <v>471</v>
       </c>
@@ -37474,7 +37474,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="305" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="20" t="s">
         <v>471</v>
       </c>
@@ -37562,7 +37562,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="20" t="s">
         <v>471</v>
       </c>
@@ -37650,7 +37650,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="307" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="20" t="s">
         <v>471</v>
       </c>
@@ -37738,7 +37738,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="20" t="s">
         <v>471</v>
       </c>
@@ -37826,7 +37826,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="309" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="20" t="s">
         <v>471</v>
       </c>
@@ -37914,7 +37914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="20" t="s">
         <v>471</v>
       </c>
@@ -38002,7 +38002,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="311" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="20" t="s">
         <v>471</v>
       </c>
@@ -38091,7 +38091,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="20" t="s">
         <v>471</v>
       </c>
@@ -38179,7 +38179,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="313" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="20" t="s">
         <v>471</v>
       </c>
@@ -38267,7 +38267,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="20" t="s">
         <v>471</v>
       </c>
@@ -38355,7 +38355,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="315" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="20" t="s">
         <v>471</v>
       </c>
@@ -38443,7 +38443,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="316" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="20" t="s">
         <v>471</v>
       </c>
@@ -38531,7 +38531,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="317" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="20" t="s">
         <v>471</v>
       </c>
@@ -38619,7 +38619,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="318" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="20" t="s">
         <v>471</v>
       </c>
@@ -38707,7 +38707,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="319" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="20" t="s">
         <v>471</v>
       </c>
@@ -38795,7 +38795,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="320" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="20" t="s">
         <v>471</v>
       </c>
@@ -38883,7 +38883,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="321" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="20" t="s">
         <v>478</v>
       </c>
@@ -38970,7 +38970,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="322" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="20" t="s">
         <v>478</v>
       </c>
@@ -39057,7 +39057,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="323" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="20" t="s">
         <v>478</v>
       </c>
@@ -39144,7 +39144,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="324" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="20" t="s">
         <v>478</v>
       </c>
@@ -39231,7 +39231,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="325" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="20" t="s">
         <v>484</v>
       </c>
@@ -39319,7 +39319,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="326" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="20" t="s">
         <v>484</v>
       </c>
@@ -39407,7 +39407,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="327" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="20" t="s">
         <v>484</v>
       </c>
@@ -39495,7 +39495,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="328" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="20" t="s">
         <v>1184</v>
       </c>
@@ -39581,7 +39581,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="329" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="20" t="s">
         <v>1184</v>
       </c>
@@ -39667,7 +39667,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="330" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="20" t="s">
         <v>1184</v>
       </c>
@@ -39753,7 +39753,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="20" t="s">
         <v>1184</v>
       </c>
@@ -39839,7 +39839,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="332" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="20" t="s">
         <v>1184</v>
       </c>
@@ -39925,7 +39925,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="333" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40011,7 +40011,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="334" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40097,7 +40097,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="335" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40183,7 +40183,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="336" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40269,7 +40269,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40355,7 +40355,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="338" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40441,7 +40441,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="339" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40527,7 +40527,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="340" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40613,7 +40613,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="341" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40699,7 +40699,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="342" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40785,7 +40785,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="343" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40871,7 +40871,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="344" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="20" t="s">
         <v>1184</v>
       </c>
@@ -40957,7 +40957,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="345" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="1" t="s">
         <v>491</v>
       </c>
@@ -41044,7 +41044,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="346" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="1" t="s">
         <v>491</v>
       </c>
@@ -41131,7 +41131,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="1" t="s">
         <v>491</v>
       </c>
@@ -41218,7 +41218,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="348" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="1" t="s">
         <v>491</v>
       </c>
@@ -41305,7 +41305,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="349" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="20" t="s">
         <v>500</v>
       </c>
@@ -41392,7 +41392,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="350" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="20" t="s">
         <v>500</v>
       </c>
@@ -41480,13 +41480,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB350">
-    <filterColumn colId="16">
-      <filters>
-        <filter val="Seasonality"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AB350"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -41507,12 +41501,12 @@
   <dimension ref="A1:AF971"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A178" activeCellId="0" sqref="A178"/>
+      <selection pane="bottomLeft" activeCell="G93" activeCellId="0" sqref="G93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="41" width="11.42"/>

</xml_diff>